<commit_message>
new csv of cfu for mike
</commit_message>
<xml_diff>
--- a/IMPAcTB_Lung_Base/IMPACTB_CFU_Base_AllDays_Lung.xlsx
+++ b/IMPAcTB_Lung_Base/IMPACTB_CFU_Base_AllDays_Lung.xlsx
@@ -5,16 +5,16 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/rstor-henao_lab/Pablo/CFU_Pipeline/IMPAcTB_Lung_Base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799225C0-45B8-0A4E-9121-17B9432FCAA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AA298B-FC9D-7449-B92A-8FBD074485FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="34840" windowHeight="22400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12120" yWindow="6140" windowWidth="22320" windowHeight="13520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="3" r:id="rId1"/>
-    <sheet name="Lung" sheetId="1" r:id="rId2"/>
+    <sheet name="metadata" sheetId="3" r:id="rId1"/>
+    <sheet name="lung" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -5799,26 +5799,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D29CD47150B3D44192901CB20E6ABB56" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6d259015367a4e5c7dcad93ba284386b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9bdb376e-ba08-4f94-9941-9e68dfd9ed35" xmlns:ns3="03c6cdc5-a326-4596-8bb5-5a108e6a189f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdf501cfd813e7d0934fe27795610cf1" ns2:_="" ns3:_="">
     <xsd:import namespace="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
@@ -6055,10 +6035,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="03c6cdc5-a326-4596-8bb5-5a108e6a189f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bdb376e-ba08-4f94-9941-9e68dfd9ed35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B5D737D-0059-4C28-A677-63B059B08D6E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D15D4F19-B157-496E-98AD-ADE72072BD25}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
+    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6075,20 +6086,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D15D4F19-B157-496E-98AD-ADE72072BD25}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B5D737D-0059-4C28-A677-63B059B08D6E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9bdb376e-ba08-4f94-9941-9e68dfd9ed35"/>
-    <ds:schemaRef ds:uri="03c6cdc5-a326-4596-8bb5-5a108e6a189f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>